<commit_message>
Sprint1 Week 1 - Test data
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-ChangeNote.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-ChangeNote.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\Falcrum_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>To</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>SPInstall</t>
+  </si>
+  <si>
+    <t>AttachDocumentName</t>
+  </si>
+  <si>
+    <t>AttachSupportDocuments</t>
+  </si>
+  <si>
+    <t>AttachSupportDocumentName</t>
+  </si>
+  <si>
+    <t>ReviewDocument</t>
+  </si>
+  <si>
+    <t>AttachDocuments</t>
   </si>
 </sst>
 </file>
@@ -486,7 +501,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,15 +513,15 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="7" max="12" width="8.5703125" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -529,19 +544,34 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -561,14 +591,14 @@
         <v>6</v>
       </c>
       <c r="G2" s="2"/>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -588,14 +618,15 @@
         <v>6</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" t="s">
+      <c r="L3" s="2"/>
+      <c r="M3" t="s">
         <v>9</v>
       </c>
-      <c r="I3" t="s">
+      <c r="N3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -615,16 +646,17 @@
         <v>6</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" t="s">
+      <c r="L4" s="2"/>
+      <c r="M4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" t="s">
+      <c r="N4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="O4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" t="s">
+      <c r="P4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the data with automation users
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-ChangeNote.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-ChangeNote.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,9 +27,6 @@
     <t>CC</t>
   </si>
   <si>
-    <t>Shaik Khaleel</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>New Transmittal from Automation</t>
   </si>
   <si>
-    <t>Anupama D. Thumrugoti</t>
-  </si>
-  <si>
     <t>TxType</t>
   </si>
   <si>
@@ -100,6 +94,12 @@
   </si>
   <si>
     <t>AttachDocuments</t>
+  </si>
+  <si>
+    <t>AutoTestAdmin</t>
+  </si>
+  <si>
+    <t>AutoTestUser</t>
   </si>
 </sst>
 </file>
@@ -529,135 +529,135 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2"/>
       <c r="M2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>